<commit_message>
New changes and complete the scrapping.py
</commit_message>
<xml_diff>
--- a/data/external/Data Taxonomy.xlsx
+++ b/data/external/Data Taxonomy.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stamatis\Desktop\MLCryptoPredictor\MLCryptoPredictor\data\external\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E8313B-6D16-49AC-A35A-CA23BCC26A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CB43FA-1FB6-4CD3-A84A-7DFEAD99DCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FRED" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FRED!$A$7:$O$17</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -354,11 +357,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -381,11 +381,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -667,10 +667,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A2:AE17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,26 +694,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
@@ -720,538 +721,545 @@
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="M7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="N7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="O7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:31" ht="403.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="8">
-        <v>45376</v>
-      </c>
-      <c r="C8" s="8">
-        <v>45376</v>
-      </c>
-      <c r="D8" s="9" t="s">
+      <c r="B8" s="7">
+        <v>45376</v>
+      </c>
+      <c r="C8" s="7">
+        <v>45376</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>41722</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <v>45373</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="L8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="M8" s="6" t="s">
+      <c r="M8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="N8" s="6">
+      <c r="N8" s="5">
         <v>83</v>
       </c>
-      <c r="O8" s="6" t="s">
+      <c r="O8" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:31" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="8">
-        <v>45376</v>
-      </c>
-      <c r="C9" s="8">
-        <v>45376</v>
-      </c>
-      <c r="D9" s="9" t="s">
+      <c r="B9" s="7">
+        <v>45376</v>
+      </c>
+      <c r="C9" s="7">
+        <v>45376</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <v>17168</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="7">
         <v>45200</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="K9" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="L9" s="6" t="s">
+      <c r="L9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="M9" s="6" t="s">
+      <c r="M9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="N9" s="6">
+      <c r="N9" s="5">
         <v>93</v>
       </c>
-      <c r="O9" s="6" t="s">
+      <c r="O9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="4"/>
-      <c r="X9" s="4"/>
-      <c r="Y9" s="4"/>
-      <c r="Z9" s="4"/>
-      <c r="AA9" s="4"/>
-      <c r="AB9" s="4"/>
-      <c r="AC9" s="4"/>
-      <c r="AD9" s="4"/>
-      <c r="AE9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="5"/>
     </row>
-    <row r="10" spans="1:31" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:31" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="8">
-        <v>45376</v>
-      </c>
-      <c r="C10" s="8">
-        <v>45376</v>
-      </c>
-      <c r="D10" s="9" t="s">
+      <c r="B10" s="7">
+        <v>45376</v>
+      </c>
+      <c r="C10" s="7">
+        <v>45376</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="7">
         <v>17168</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="7">
         <v>45200</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="J10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="L10" s="6" t="s">
+      <c r="L10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="M10" s="6" t="s">
+      <c r="M10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="N10" s="6">
+      <c r="N10" s="5">
         <v>92</v>
       </c>
-      <c r="O10" s="6" t="s">
+      <c r="O10" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:31" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="8">
-        <v>45376</v>
-      </c>
-      <c r="C11" s="8">
-        <v>45376</v>
-      </c>
-      <c r="D11" s="9" t="s">
+      <c r="B11" s="7">
+        <v>45376</v>
+      </c>
+      <c r="C11" s="7">
+        <v>45376</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="7">
         <v>17533</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="7">
         <v>45323</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="I11" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="J11" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="K11" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="L11" s="6" t="s">
+      <c r="L11" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="M11" s="6" t="s">
+      <c r="M11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="N11" s="6">
+      <c r="N11" s="5">
         <v>95</v>
       </c>
-      <c r="O11" s="6" t="s">
+      <c r="O11" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:31" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="8">
-        <v>45376</v>
-      </c>
-      <c r="C12" s="8">
-        <v>45376</v>
-      </c>
-      <c r="D12" s="9" t="s">
+      <c r="B12" s="7">
+        <v>45376</v>
+      </c>
+      <c r="C12" s="7">
+        <v>45376</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="7">
         <v>17168</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="7">
         <v>45323</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J12" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="K12" s="11" t="s">
+      <c r="K12" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="L12" s="6" t="s">
+      <c r="L12" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="M12" s="6" t="s">
+      <c r="M12" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="N12" s="6">
+      <c r="N12" s="5">
         <v>95</v>
       </c>
-      <c r="O12" s="6" t="s">
+      <c r="O12" s="5" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:31" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="8">
-        <v>45376</v>
-      </c>
-      <c r="C13" s="8">
-        <v>45376</v>
-      </c>
-      <c r="D13" s="9" t="s">
+      <c r="B13" s="7">
+        <v>45376</v>
+      </c>
+      <c r="C13" s="7">
+        <v>45376</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="7">
         <v>27912</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="7">
         <v>45373</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="I13" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="J13" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="K13" s="11" t="s">
+      <c r="K13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="L13" s="6" t="s">
+      <c r="L13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="M13" s="6" t="s">
+      <c r="M13" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N13" s="6">
+      <c r="N13" s="5">
         <v>100</v>
       </c>
-      <c r="O13" s="6" t="s">
+      <c r="O13" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:31" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="8">
-        <v>45376</v>
-      </c>
-      <c r="C14" s="8">
-        <v>45376</v>
-      </c>
-      <c r="D14" s="9" t="s">
+      <c r="B14" s="7">
+        <v>45376</v>
+      </c>
+      <c r="C14" s="7">
+        <v>45376</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="7">
         <v>29952</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="7">
         <v>45352</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="I14" s="11" t="s">
+      <c r="I14" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="J14" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="K14" s="11" t="s">
+      <c r="K14" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="L14" s="6" t="s">
+      <c r="L14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="M14" s="6" t="s">
+      <c r="M14" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="N14" s="6">
+      <c r="N14" s="5">
         <v>80</v>
       </c>
-      <c r="O14" s="6" t="s">
+      <c r="O14" s="5" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:31" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="8">
-        <v>45376</v>
-      </c>
-      <c r="C15" s="8">
-        <v>45376</v>
-      </c>
-      <c r="D15" s="9" t="s">
+      <c r="B15" s="7">
+        <v>45376</v>
+      </c>
+      <c r="C15" s="7">
+        <v>45376</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="7">
         <v>37623</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="7">
         <v>45373</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I15" s="11" t="s">
+      <c r="I15" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="J15" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="K15" s="11" t="s">
+      <c r="K15" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="L15" s="6" t="s">
+      <c r="L15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="M15" s="6" t="s">
+      <c r="M15" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="N15" s="6">
+      <c r="N15" s="5">
         <v>89</v>
       </c>
-      <c r="O15" s="6" t="s">
+      <c r="O15" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
+    <row r="16" spans="1:31" ht="172.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="8">
-        <v>45376</v>
-      </c>
-      <c r="C16" s="8">
-        <v>45376</v>
-      </c>
-      <c r="D16" s="9" t="s">
+      <c r="B16" s="7">
+        <v>45376</v>
+      </c>
+      <c r="C16" s="7">
+        <v>45376</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="7">
         <v>24838</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="7">
         <v>45323</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="I16" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="J16" s="6" t="s">
+      <c r="J16" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="K16" s="11" t="s">
+      <c r="K16" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="L16" s="6" t="s">
+      <c r="L16" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="M16" s="6" t="s">
+      <c r="M16" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="N16" s="6">
+      <c r="N16" s="5">
         <v>84</v>
       </c>
-      <c r="O16" s="6" t="s">
+      <c r="O16" s="5" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="273.60000000000002" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="8">
-        <v>45376</v>
-      </c>
-      <c r="C17" s="8">
-        <v>45376</v>
-      </c>
-      <c r="D17" s="9" t="s">
+      <c r="B17" s="7">
+        <v>45376</v>
+      </c>
+      <c r="C17" s="7">
+        <v>45376</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="7">
         <v>29528</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="7">
         <v>45327</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="I17" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="J17" s="6" t="s">
+      <c r="J17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K17" s="11" t="s">
+      <c r="K17" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="L17" s="6" t="s">
+      <c r="L17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="M17" s="6" t="s">
+      <c r="M17" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="N17" s="6">
+      <c r="N17" s="5">
         <v>87</v>
       </c>
-      <c r="O17" s="6" t="s">
+      <c r="O17" s="5" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A7:O17" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="10">
+      <filters>
+        <filter val="Not Seasonally Adjusted"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A2:O2"/>
   </mergeCells>

</xml_diff>